<commit_message>
Ordner Hardware hinzugefuegt. Schema wurde erstellt.
</commit_message>
<xml_diff>
--- a/Documents/BOM_LightDimmer.xlsx
+++ b/Documents/BOM_LightDimmer.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\Local Git Repository\RemoteDimmer\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="672" yWindow="36" windowWidth="15828" windowHeight="6576"/>
+    <workbookView xWindow="675" yWindow="30" windowWidth="15825" windowHeight="6570"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -162,8 +167,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,18 +238,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -282,9 +295,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,9 +329,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,9 +381,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -525,21 +574,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="7" max="7" width="92.33203125" customWidth="1"/>
+    <col min="7" max="7" width="92.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -562,7 +611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -583,7 +632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -604,7 +653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
@@ -625,7 +674,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
@@ -646,7 +695,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -661,7 +710,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -676,7 +725,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -699,7 +748,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -722,7 +771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -739,7 +788,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -762,7 +811,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -785,7 +834,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
@@ -806,7 +855,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
@@ -827,7 +876,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -854,24 +903,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>